<commit_message>
Added ggCS algorithm - doesn't work yet
</commit_message>
<xml_diff>
--- a/processed_input_data_bomv1.xlsx
+++ b/processed_input_data_bomv1.xlsx
@@ -438,37 +438,37 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2">
-        <v>3.625</v>
+        <v>3625</v>
       </c>
       <c r="B2">
         <v>40</v>
       </c>
       <c r="C2">
-        <v>3.625</v>
+        <v>3625</v>
       </c>
       <c r="D2">
         <v>40</v>
       </c>
       <c r="E2">
-        <v>3.625</v>
+        <v>3625</v>
       </c>
       <c r="F2">
         <v>40</v>
       </c>
       <c r="G2">
-        <v>6.125</v>
+        <v>6125</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2">
-        <v>6.125</v>
+        <v>6125</v>
       </c>
       <c r="J2">
         <v>2</v>
       </c>
       <c r="K2">
-        <v>6.125</v>
+        <v>6125</v>
       </c>
       <c r="L2">
         <v>2</v>
@@ -476,37 +476,37 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3">
-        <v>5.875</v>
+        <v>5875</v>
       </c>
       <c r="B3">
         <v>6</v>
       </c>
       <c r="C3">
-        <v>5.875</v>
+        <v>5875</v>
       </c>
       <c r="D3">
         <v>6</v>
       </c>
       <c r="E3">
-        <v>5.875</v>
+        <v>5875</v>
       </c>
       <c r="F3">
         <v>6</v>
       </c>
       <c r="G3">
-        <v>7.755</v>
+        <v>7755</v>
       </c>
       <c r="H3">
         <v>69</v>
       </c>
       <c r="I3">
-        <v>7.755</v>
+        <v>7755</v>
       </c>
       <c r="J3">
         <v>69</v>
       </c>
       <c r="K3">
-        <v>7.755</v>
+        <v>7755</v>
       </c>
       <c r="L3">
         <v>69</v>
@@ -514,37 +514,37 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
-        <v>6.095</v>
+        <v>6095</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
       <c r="C4">
-        <v>6.095</v>
+        <v>6095</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4">
-        <v>6.095</v>
+        <v>6095</v>
       </c>
       <c r="F4">
         <v>10</v>
       </c>
       <c r="G4">
-        <v>12.125</v>
+        <v>12125</v>
       </c>
       <c r="H4">
         <v>7</v>
       </c>
       <c r="I4">
-        <v>12.125</v>
+        <v>12125</v>
       </c>
       <c r="J4">
         <v>7</v>
       </c>
       <c r="K4">
-        <v>12.125</v>
+        <v>12125</v>
       </c>
       <c r="L4">
         <v>7</v>
@@ -552,37 +552,37 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
-        <v>9.904999999999999</v>
+        <v>9905</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
       <c r="C5">
-        <v>9.904999999999999</v>
+        <v>9905</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
       <c r="E5">
-        <v>9.904999999999999</v>
+        <v>9905</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
       <c r="G5">
-        <v>14.625</v>
+        <v>14625</v>
       </c>
       <c r="H5">
         <v>22</v>
       </c>
       <c r="I5">
-        <v>14.625</v>
+        <v>14625</v>
       </c>
       <c r="J5">
         <v>22</v>
       </c>
       <c r="K5">
-        <v>14.625</v>
+        <v>14625</v>
       </c>
       <c r="L5">
         <v>22</v>
@@ -590,37 +590,37 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6">
-        <v>10.375</v>
+        <v>10375</v>
       </c>
       <c r="B6">
         <v>20</v>
       </c>
       <c r="C6">
-        <v>10.375</v>
+        <v>10375</v>
       </c>
       <c r="D6">
         <v>20</v>
       </c>
       <c r="E6">
-        <v>10.375</v>
+        <v>10375</v>
       </c>
       <c r="F6">
         <v>20</v>
       </c>
       <c r="G6">
-        <v>16.625</v>
+        <v>16625</v>
       </c>
       <c r="H6">
         <v>27</v>
       </c>
       <c r="I6">
-        <v>16.625</v>
+        <v>16625</v>
       </c>
       <c r="J6">
         <v>27</v>
       </c>
       <c r="K6">
-        <v>16.625</v>
+        <v>16625</v>
       </c>
       <c r="L6">
         <v>27</v>
@@ -628,37 +628,37 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7">
-        <v>11.185</v>
+        <v>11185</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7">
-        <v>11.185</v>
+        <v>11185</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7">
-        <v>11.185</v>
+        <v>11185</v>
       </c>
       <c r="F7">
         <v>5</v>
       </c>
       <c r="G7">
-        <v>20.375</v>
+        <v>20375</v>
       </c>
       <c r="H7">
         <v>66</v>
       </c>
       <c r="I7">
-        <v>20.375</v>
+        <v>20375</v>
       </c>
       <c r="J7">
         <v>66</v>
       </c>
       <c r="K7">
-        <v>20.375</v>
+        <v>20375</v>
       </c>
       <c r="L7">
         <v>66</v>
@@ -666,37 +666,37 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8">
-        <v>13.125</v>
+        <v>13125</v>
       </c>
       <c r="B8">
         <v>24</v>
       </c>
       <c r="C8">
-        <v>13.125</v>
+        <v>13125</v>
       </c>
       <c r="D8">
         <v>24</v>
       </c>
       <c r="E8">
-        <v>13.125</v>
+        <v>13125</v>
       </c>
       <c r="F8">
         <v>24</v>
       </c>
       <c r="G8">
-        <v>21.875</v>
+        <v>21875</v>
       </c>
       <c r="H8">
         <v>82</v>
       </c>
       <c r="I8">
-        <v>21.875</v>
+        <v>21875</v>
       </c>
       <c r="J8">
         <v>82</v>
       </c>
       <c r="K8">
-        <v>21.875</v>
+        <v>21875</v>
       </c>
       <c r="L8">
         <v>82</v>
@@ -704,37 +704,37 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9">
-        <v>15.595</v>
+        <v>15595</v>
       </c>
       <c r="B9">
         <v>5</v>
       </c>
       <c r="C9">
-        <v>15.595</v>
+        <v>15595</v>
       </c>
       <c r="D9">
         <v>5</v>
       </c>
       <c r="E9">
-        <v>15.595</v>
+        <v>15595</v>
       </c>
       <c r="F9">
         <v>5</v>
       </c>
       <c r="G9">
-        <v>41.125</v>
+        <v>41125</v>
       </c>
       <c r="H9">
         <v>47</v>
       </c>
       <c r="I9">
-        <v>41.125</v>
+        <v>41125</v>
       </c>
       <c r="J9">
         <v>47</v>
       </c>
       <c r="K9">
-        <v>41.125</v>
+        <v>41125</v>
       </c>
       <c r="L9">
         <v>47</v>
@@ -742,37 +742,37 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10">
-        <v>32.125</v>
+        <v>32125</v>
       </c>
       <c r="B10">
         <v>20</v>
       </c>
       <c r="C10">
-        <v>32.125</v>
+        <v>32125</v>
       </c>
       <c r="D10">
         <v>20</v>
       </c>
       <c r="E10">
-        <v>32.125</v>
+        <v>32125</v>
       </c>
       <c r="F10">
         <v>20</v>
       </c>
       <c r="G10">
-        <v>48.125</v>
+        <v>48125</v>
       </c>
       <c r="H10">
         <v>27</v>
       </c>
       <c r="I10">
-        <v>48.125</v>
+        <v>48125</v>
       </c>
       <c r="J10">
         <v>27</v>
       </c>
       <c r="K10">
-        <v>48.125</v>
+        <v>48125</v>
       </c>
       <c r="L10">
         <v>27</v>
@@ -780,37 +780,37 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11">
-        <v>41.125</v>
+        <v>41125</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>41.125</v>
+        <v>41125</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>41.125</v>
+        <v>41125</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11">
-        <v>60.125</v>
+        <v>60125</v>
       </c>
       <c r="H11">
         <v>18</v>
       </c>
       <c r="I11">
-        <v>60.125</v>
+        <v>60125</v>
       </c>
       <c r="J11">
         <v>18</v>
       </c>
       <c r="K11">
-        <v>60.125</v>
+        <v>60125</v>
       </c>
       <c r="L11">
         <v>18</v>
@@ -818,37 +818,37 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12">
-        <v>42.625</v>
+        <v>42625</v>
       </c>
       <c r="B12">
         <v>3</v>
       </c>
       <c r="C12">
-        <v>42.625</v>
+        <v>42625</v>
       </c>
       <c r="D12">
         <v>3</v>
       </c>
       <c r="E12">
-        <v>42.625</v>
+        <v>42625</v>
       </c>
       <c r="F12">
         <v>3</v>
       </c>
       <c r="G12">
-        <v>62.125</v>
+        <v>62125</v>
       </c>
       <c r="H12">
         <v>5</v>
       </c>
       <c r="I12">
-        <v>62.125</v>
+        <v>62125</v>
       </c>
       <c r="J12">
         <v>5</v>
       </c>
       <c r="K12">
-        <v>62.125</v>
+        <v>62125</v>
       </c>
       <c r="L12">
         <v>5</v>
@@ -856,37 +856,37 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13">
-        <v>45.625</v>
+        <v>45625</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13">
-        <v>45.625</v>
+        <v>45625</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13">
-        <v>45.625</v>
+        <v>45625</v>
       </c>
       <c r="F13">
         <v>3</v>
       </c>
       <c r="G13">
-        <v>79.625</v>
+        <v>79625</v>
       </c>
       <c r="H13">
         <v>2</v>
       </c>
       <c r="I13">
-        <v>79.625</v>
+        <v>79625</v>
       </c>
       <c r="J13">
         <v>2</v>
       </c>
       <c r="K13">
-        <v>79.625</v>
+        <v>79625</v>
       </c>
       <c r="L13">
         <v>2</v>
@@ -894,37 +894,37 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14">
-        <v>51.215</v>
+        <v>51215</v>
       </c>
       <c r="B14">
         <v>5</v>
       </c>
       <c r="C14">
-        <v>51.215</v>
+        <v>51215</v>
       </c>
       <c r="D14">
         <v>5</v>
       </c>
       <c r="E14">
-        <v>51.215</v>
+        <v>51215</v>
       </c>
       <c r="F14">
         <v>5</v>
       </c>
       <c r="G14">
-        <v>86.125</v>
+        <v>86125</v>
       </c>
       <c r="H14">
         <v>25</v>
       </c>
       <c r="I14">
-        <v>86.125</v>
+        <v>86125</v>
       </c>
       <c r="J14">
         <v>25</v>
       </c>
       <c r="K14">
-        <v>86.125</v>
+        <v>86125</v>
       </c>
       <c r="L14">
         <v>25</v>
@@ -932,37 +932,37 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15">
-        <v>62.125</v>
+        <v>62125</v>
       </c>
       <c r="B15">
         <v>15</v>
       </c>
       <c r="C15">
-        <v>62.125</v>
+        <v>62125</v>
       </c>
       <c r="D15">
         <v>15</v>
       </c>
       <c r="E15">
-        <v>62.125</v>
+        <v>62125</v>
       </c>
       <c r="F15">
         <v>15</v>
       </c>
       <c r="G15">
-        <v>92.755</v>
+        <v>92755</v>
       </c>
       <c r="H15">
         <v>161</v>
       </c>
       <c r="I15">
-        <v>92.755</v>
+        <v>92755</v>
       </c>
       <c r="J15">
         <v>161</v>
       </c>
       <c r="K15">
-        <v>92.755</v>
+        <v>92755</v>
       </c>
       <c r="L15">
         <v>161</v>
@@ -970,37 +970,37 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16">
-        <v>81.625</v>
+        <v>81625</v>
       </c>
       <c r="B16">
         <v>16</v>
       </c>
       <c r="C16">
-        <v>81.625</v>
+        <v>81625</v>
       </c>
       <c r="D16">
         <v>16</v>
       </c>
       <c r="E16">
-        <v>81.625</v>
+        <v>81625</v>
       </c>
       <c r="F16">
         <v>16</v>
       </c>
       <c r="G16">
-        <v>96.125</v>
+        <v>96125</v>
       </c>
       <c r="H16">
         <v>51</v>
       </c>
       <c r="I16">
-        <v>96.125</v>
+        <v>96125</v>
       </c>
       <c r="J16">
         <v>51</v>
       </c>
       <c r="K16">
-        <v>96</v>
+        <v>96000</v>
       </c>
       <c r="L16">
         <v>51</v>
@@ -1008,31 +1008,31 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17">
-        <v>86.125</v>
+        <v>86125</v>
       </c>
       <c r="B17">
         <v>55</v>
       </c>
       <c r="C17">
-        <v>86.125</v>
+        <v>86125</v>
       </c>
       <c r="D17">
         <v>55</v>
       </c>
       <c r="E17">
-        <v>86.125</v>
+        <v>86125</v>
       </c>
       <c r="F17">
         <v>55</v>
       </c>
       <c r="G17">
-        <v>120.125</v>
+        <v>120125</v>
       </c>
       <c r="H17">
         <v>2</v>
       </c>
       <c r="I17">
-        <v>120.125</v>
+        <v>120125</v>
       </c>
       <c r="J17">
         <v>2</v>
@@ -1040,19 +1040,19 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
-        <v>92.755</v>
+        <v>92755</v>
       </c>
       <c r="B18">
         <v>18</v>
       </c>
       <c r="C18">
-        <v>92.755</v>
+        <v>92755</v>
       </c>
       <c r="D18">
         <v>18</v>
       </c>
       <c r="E18">
-        <v>92.755</v>
+        <v>92755</v>
       </c>
       <c r="F18">
         <v>18</v>
@@ -1060,19 +1060,19 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19">
-        <v>96.125</v>
+        <v>96125</v>
       </c>
       <c r="B19">
         <v>71</v>
       </c>
       <c r="C19">
-        <v>96.125</v>
+        <v>96125</v>
       </c>
       <c r="D19">
         <v>71</v>
       </c>
       <c r="E19">
-        <v>96</v>
+        <v>96000</v>
       </c>
       <c r="F19">
         <v>71</v>

</xml_diff>

<commit_message>
Added pywrap ortools algorithm - also doesnt work. need to debug both
</commit_message>
<xml_diff>
--- a/processed_input_data_bomv1.xlsx
+++ b/processed_input_data_bomv1.xlsx
@@ -438,37 +438,37 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2">
-        <v>3625</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>40</v>
       </c>
       <c r="C2">
-        <v>3625</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>40</v>
       </c>
       <c r="E2">
-        <v>3625</v>
+        <v>4</v>
       </c>
       <c r="F2">
         <v>40</v>
       </c>
       <c r="G2">
-        <v>6125</v>
+        <v>6</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2">
-        <v>6125</v>
+        <v>6</v>
       </c>
       <c r="J2">
         <v>2</v>
       </c>
       <c r="K2">
-        <v>6125</v>
+        <v>6</v>
       </c>
       <c r="L2">
         <v>2</v>
@@ -476,37 +476,37 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3">
-        <v>5875</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>6</v>
       </c>
       <c r="C3">
-        <v>5875</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>6</v>
       </c>
       <c r="E3">
-        <v>5875</v>
+        <v>6</v>
       </c>
       <c r="F3">
         <v>6</v>
       </c>
       <c r="G3">
-        <v>7755</v>
+        <v>8</v>
       </c>
       <c r="H3">
         <v>69</v>
       </c>
       <c r="I3">
-        <v>7755</v>
+        <v>8</v>
       </c>
       <c r="J3">
         <v>69</v>
       </c>
       <c r="K3">
-        <v>7755</v>
+        <v>8</v>
       </c>
       <c r="L3">
         <v>69</v>
@@ -514,37 +514,37 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
-        <v>6095</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
       <c r="C4">
-        <v>6095</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4">
-        <v>6095</v>
+        <v>6</v>
       </c>
       <c r="F4">
         <v>10</v>
       </c>
       <c r="G4">
-        <v>12125</v>
+        <v>12</v>
       </c>
       <c r="H4">
         <v>7</v>
       </c>
       <c r="I4">
-        <v>12125</v>
+        <v>12</v>
       </c>
       <c r="J4">
         <v>7</v>
       </c>
       <c r="K4">
-        <v>12125</v>
+        <v>12</v>
       </c>
       <c r="L4">
         <v>7</v>
@@ -552,37 +552,37 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
-        <v>9905</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
       <c r="C5">
-        <v>9905</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
       <c r="E5">
-        <v>9905</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
       <c r="G5">
-        <v>14625</v>
+        <v>14</v>
       </c>
       <c r="H5">
         <v>22</v>
       </c>
       <c r="I5">
-        <v>14625</v>
+        <v>14</v>
       </c>
       <c r="J5">
         <v>22</v>
       </c>
       <c r="K5">
-        <v>14625</v>
+        <v>14</v>
       </c>
       <c r="L5">
         <v>22</v>
@@ -590,37 +590,37 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6">
-        <v>10375</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>20</v>
       </c>
       <c r="C6">
-        <v>10375</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>20</v>
       </c>
       <c r="E6">
-        <v>10375</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>20</v>
       </c>
       <c r="G6">
-        <v>16625</v>
+        <v>16</v>
       </c>
       <c r="H6">
         <v>27</v>
       </c>
       <c r="I6">
-        <v>16625</v>
+        <v>16</v>
       </c>
       <c r="J6">
         <v>27</v>
       </c>
       <c r="K6">
-        <v>16625</v>
+        <v>16</v>
       </c>
       <c r="L6">
         <v>27</v>
@@ -628,37 +628,37 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7">
-        <v>11185</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7">
-        <v>11185</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7">
-        <v>11185</v>
+        <v>11</v>
       </c>
       <c r="F7">
         <v>5</v>
       </c>
       <c r="G7">
-        <v>20375</v>
+        <v>20</v>
       </c>
       <c r="H7">
         <v>66</v>
       </c>
       <c r="I7">
-        <v>20375</v>
+        <v>20</v>
       </c>
       <c r="J7">
         <v>66</v>
       </c>
       <c r="K7">
-        <v>20375</v>
+        <v>20</v>
       </c>
       <c r="L7">
         <v>66</v>
@@ -666,37 +666,37 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8">
-        <v>13125</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>24</v>
       </c>
       <c r="C8">
-        <v>13125</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>24</v>
       </c>
       <c r="E8">
-        <v>13125</v>
+        <v>13</v>
       </c>
       <c r="F8">
         <v>24</v>
       </c>
       <c r="G8">
-        <v>21875</v>
+        <v>22</v>
       </c>
       <c r="H8">
         <v>82</v>
       </c>
       <c r="I8">
-        <v>21875</v>
+        <v>22</v>
       </c>
       <c r="J8">
         <v>82</v>
       </c>
       <c r="K8">
-        <v>21875</v>
+        <v>22</v>
       </c>
       <c r="L8">
         <v>82</v>
@@ -704,37 +704,37 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9">
-        <v>15595</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>5</v>
       </c>
       <c r="C9">
-        <v>15595</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>5</v>
       </c>
       <c r="E9">
-        <v>15595</v>
+        <v>15</v>
       </c>
       <c r="F9">
         <v>5</v>
       </c>
       <c r="G9">
-        <v>41125</v>
+        <v>41</v>
       </c>
       <c r="H9">
         <v>47</v>
       </c>
       <c r="I9">
-        <v>41125</v>
+        <v>41</v>
       </c>
       <c r="J9">
         <v>47</v>
       </c>
       <c r="K9">
-        <v>41125</v>
+        <v>41</v>
       </c>
       <c r="L9">
         <v>47</v>
@@ -742,37 +742,37 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10">
-        <v>32125</v>
+        <v>32</v>
       </c>
       <c r="B10">
         <v>20</v>
       </c>
       <c r="C10">
-        <v>32125</v>
+        <v>32</v>
       </c>
       <c r="D10">
         <v>20</v>
       </c>
       <c r="E10">
-        <v>32125</v>
+        <v>32</v>
       </c>
       <c r="F10">
         <v>20</v>
       </c>
       <c r="G10">
-        <v>48125</v>
+        <v>48</v>
       </c>
       <c r="H10">
         <v>27</v>
       </c>
       <c r="I10">
-        <v>48125</v>
+        <v>48</v>
       </c>
       <c r="J10">
         <v>27</v>
       </c>
       <c r="K10">
-        <v>48125</v>
+        <v>48</v>
       </c>
       <c r="L10">
         <v>27</v>
@@ -780,37 +780,37 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11">
-        <v>41125</v>
+        <v>41</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>41125</v>
+        <v>41</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>41125</v>
+        <v>41</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11">
-        <v>60125</v>
+        <v>60</v>
       </c>
       <c r="H11">
         <v>18</v>
       </c>
       <c r="I11">
-        <v>60125</v>
+        <v>60</v>
       </c>
       <c r="J11">
         <v>18</v>
       </c>
       <c r="K11">
-        <v>60125</v>
+        <v>60</v>
       </c>
       <c r="L11">
         <v>18</v>
@@ -818,37 +818,37 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12">
-        <v>42625</v>
+        <v>42</v>
       </c>
       <c r="B12">
         <v>3</v>
       </c>
       <c r="C12">
-        <v>42625</v>
+        <v>42</v>
       </c>
       <c r="D12">
         <v>3</v>
       </c>
       <c r="E12">
-        <v>42625</v>
+        <v>42</v>
       </c>
       <c r="F12">
         <v>3</v>
       </c>
       <c r="G12">
-        <v>62125</v>
+        <v>62</v>
       </c>
       <c r="H12">
         <v>5</v>
       </c>
       <c r="I12">
-        <v>62125</v>
+        <v>62</v>
       </c>
       <c r="J12">
         <v>5</v>
       </c>
       <c r="K12">
-        <v>62125</v>
+        <v>62</v>
       </c>
       <c r="L12">
         <v>5</v>
@@ -856,37 +856,37 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13">
-        <v>45625</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13">
-        <v>45625</v>
+        <v>46</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13">
-        <v>45625</v>
+        <v>46</v>
       </c>
       <c r="F13">
         <v>3</v>
       </c>
       <c r="G13">
-        <v>79625</v>
+        <v>80</v>
       </c>
       <c r="H13">
         <v>2</v>
       </c>
       <c r="I13">
-        <v>79625</v>
+        <v>80</v>
       </c>
       <c r="J13">
         <v>2</v>
       </c>
       <c r="K13">
-        <v>79625</v>
+        <v>80</v>
       </c>
       <c r="L13">
         <v>2</v>
@@ -894,37 +894,37 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14">
-        <v>51215</v>
+        <v>51</v>
       </c>
       <c r="B14">
         <v>5</v>
       </c>
       <c r="C14">
-        <v>51215</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <v>5</v>
       </c>
       <c r="E14">
-        <v>51215</v>
+        <v>51</v>
       </c>
       <c r="F14">
         <v>5</v>
       </c>
       <c r="G14">
-        <v>86125</v>
+        <v>86</v>
       </c>
       <c r="H14">
         <v>25</v>
       </c>
       <c r="I14">
-        <v>86125</v>
+        <v>86</v>
       </c>
       <c r="J14">
         <v>25</v>
       </c>
       <c r="K14">
-        <v>86125</v>
+        <v>86</v>
       </c>
       <c r="L14">
         <v>25</v>
@@ -932,37 +932,37 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15">
-        <v>62125</v>
+        <v>62</v>
       </c>
       <c r="B15">
         <v>15</v>
       </c>
       <c r="C15">
-        <v>62125</v>
+        <v>62</v>
       </c>
       <c r="D15">
         <v>15</v>
       </c>
       <c r="E15">
-        <v>62125</v>
+        <v>62</v>
       </c>
       <c r="F15">
         <v>15</v>
       </c>
       <c r="G15">
-        <v>92755</v>
+        <v>93</v>
       </c>
       <c r="H15">
         <v>161</v>
       </c>
       <c r="I15">
-        <v>92755</v>
+        <v>93</v>
       </c>
       <c r="J15">
         <v>161</v>
       </c>
       <c r="K15">
-        <v>92755</v>
+        <v>93</v>
       </c>
       <c r="L15">
         <v>161</v>
@@ -970,37 +970,37 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16">
-        <v>81625</v>
+        <v>82</v>
       </c>
       <c r="B16">
         <v>16</v>
       </c>
       <c r="C16">
-        <v>81625</v>
+        <v>82</v>
       </c>
       <c r="D16">
         <v>16</v>
       </c>
       <c r="E16">
-        <v>81625</v>
+        <v>82</v>
       </c>
       <c r="F16">
         <v>16</v>
       </c>
       <c r="G16">
-        <v>96125</v>
+        <v>96</v>
       </c>
       <c r="H16">
         <v>51</v>
       </c>
       <c r="I16">
-        <v>96125</v>
+        <v>96</v>
       </c>
       <c r="J16">
         <v>51</v>
       </c>
       <c r="K16">
-        <v>96000</v>
+        <v>96</v>
       </c>
       <c r="L16">
         <v>51</v>
@@ -1008,31 +1008,31 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17">
-        <v>86125</v>
+        <v>86</v>
       </c>
       <c r="B17">
         <v>55</v>
       </c>
       <c r="C17">
-        <v>86125</v>
+        <v>86</v>
       </c>
       <c r="D17">
         <v>55</v>
       </c>
       <c r="E17">
-        <v>86125</v>
+        <v>86</v>
       </c>
       <c r="F17">
         <v>55</v>
       </c>
       <c r="G17">
-        <v>120125</v>
+        <v>120</v>
       </c>
       <c r="H17">
         <v>2</v>
       </c>
       <c r="I17">
-        <v>120125</v>
+        <v>120</v>
       </c>
       <c r="J17">
         <v>2</v>
@@ -1040,19 +1040,19 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
-        <v>92755</v>
+        <v>93</v>
       </c>
       <c r="B18">
         <v>18</v>
       </c>
       <c r="C18">
-        <v>92755</v>
+        <v>93</v>
       </c>
       <c r="D18">
         <v>18</v>
       </c>
       <c r="E18">
-        <v>92755</v>
+        <v>93</v>
       </c>
       <c r="F18">
         <v>18</v>
@@ -1060,19 +1060,19 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19">
-        <v>96125</v>
+        <v>96</v>
       </c>
       <c r="B19">
         <v>71</v>
       </c>
       <c r="C19">
-        <v>96125</v>
+        <v>96</v>
       </c>
       <c r="D19">
         <v>71</v>
       </c>
       <c r="E19">
-        <v>96000</v>
+        <v>96</v>
       </c>
       <c r="F19">
         <v>71</v>

</xml_diff>